<commit_message>
Fluxo carga fracionada xlsx terminado
Os fluxos que tratam o cenário de cargas fracionadas com entradas em xlsx, e.g. Onofre, foram terminados e testados com sucesso.
</commit_message>
<xml_diff>
--- a/ep_freight_table.xlsx
+++ b/ep_freight_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BlueShift075\Documents\GitHub\Intelipost-Media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{68530AC9-9588-4F81-B671-8D55F485FC01}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36"/>
+  <xr:revisionPtr documentId="13_ncr:1_{E9482985-378B-4C6B-B58B-908976AA4E04}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36"/>
   <bookViews>
     <workbookView windowHeight="9600" windowWidth="12800" xWindow="240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="120"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="65">
   <si>
     <t>destination_geographic_identifier</t>
   </si>
@@ -200,6 +200,21 @@
   </si>
   <si>
     <t>SP-Interior 3</t>
+  </si>
+  <si>
+    <t>range_end</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>100</t>
   </si>
 </sst>
 </file>
@@ -554,15 +569,20 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>range_end</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>base_freight_cost</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>percentage_invoice</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>exceeding_weight_cost</t>
         </is>
@@ -576,10 +596,15 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>37,49</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>0,30</t>
         </is>
@@ -593,10 +618,15 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>44,11</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>0,30</t>
         </is>
@@ -610,10 +640,15 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>46,57</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>0,30</t>
         </is>
@@ -627,15 +662,20 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>56,35</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>0,30</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>0,46</t>
         </is>
@@ -649,10 +689,15 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>49,69</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>0,40</t>
         </is>
@@ -666,10 +711,15 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>58,46</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>0,40</t>
         </is>
@@ -683,10 +733,15 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>63,00</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>0,40</t>
         </is>
@@ -700,15 +755,20 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>72,04</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>0,40</t>
-        </is>
-      </c>
       <c r="D9" t="inlineStr">
+        <is>
+          <t>0,40</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>0,53</t>
         </is>
@@ -722,10 +782,15 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
           <t>49,69</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>0,40</t>
         </is>
@@ -739,10 +804,15 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
           <t>58,46</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>0,40</t>
         </is>
@@ -756,10 +826,15 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
           <t>63,00</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>0,40</t>
         </is>
@@ -773,15 +848,20 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
           <t>72,04</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>0,40</t>
-        </is>
-      </c>
       <c r="D13" t="inlineStr">
+        <is>
+          <t>0,40</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
         <is>
           <t>0,53</t>
         </is>
@@ -795,10 +875,15 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
           <t>65,69</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>0,40</t>
         </is>
@@ -812,10 +897,15 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
           <t>77,28</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>0,40</t>
         </is>
@@ -829,10 +919,15 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
           <t>82,43</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>0,40</t>
         </is>
@@ -846,15 +941,20 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
           <t>92,74</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>0,40</t>
-        </is>
-      </c>
       <c r="D17" t="inlineStr">
+        <is>
+          <t>0,40</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
         <is>
           <t>0,77</t>
         </is>
@@ -868,10 +968,15 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
           <t>98,79</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>0,60</t>
         </is>
@@ -885,10 +990,15 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
           <t>116,23</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>0,60</t>
         </is>
@@ -902,10 +1012,15 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
           <t>121,18</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>0,60</t>
         </is>
@@ -919,15 +1034,20 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
           <t>136,01</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>0,60</t>
-        </is>
-      </c>
       <c r="D21" t="inlineStr">
+        <is>
+          <t>0,60</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
         <is>
           <t>1,24</t>
         </is>
@@ -941,10 +1061,15 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
           <t>45,69</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>0,40</t>
         </is>
@@ -958,10 +1083,15 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
           <t>53,75</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>0,40</t>
         </is>
@@ -975,10 +1105,15 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
           <t>63,99</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>0,40</t>
         </is>
@@ -992,15 +1127,20 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
           <t>74,56</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>0,40</t>
-        </is>
-      </c>
       <c r="D25" t="inlineStr">
+        <is>
+          <t>0,40</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
         <is>
           <t>0,49</t>
         </is>
@@ -1014,10 +1154,15 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
           <t>45,69</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>0,40</t>
         </is>
@@ -1031,10 +1176,15 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
           <t>53,75</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="D27" t="inlineStr">
         <is>
           <t>0,40</t>
         </is>
@@ -1048,10 +1198,15 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
           <t>63,99</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t>0,40</t>
         </is>
@@ -1065,15 +1220,20 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
           <t>74,56</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>0,40</t>
-        </is>
-      </c>
       <c r="D29" t="inlineStr">
+        <is>
+          <t>0,40</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
         <is>
           <t>0,49</t>
         </is>
@@ -1087,10 +1247,15 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
           <t>46,82</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="D30" t="inlineStr">
         <is>
           <t>0,60</t>
         </is>
@@ -1104,10 +1269,15 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
           <t>55,08</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="D31" t="inlineStr">
         <is>
           <t>0,60</t>
         </is>
@@ -1121,10 +1291,15 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
           <t>70,21</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t>0,60</t>
         </is>
@@ -1138,15 +1313,20 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
           <t>76,51</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>0,60</t>
-        </is>
-      </c>
       <c r="D33" t="inlineStr">
+        <is>
+          <t>0,60</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
         <is>
           <t>0,56</t>
         </is>
@@ -1160,10 +1340,15 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
           <t>46,82</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="D34" t="inlineStr">
         <is>
           <t>0,60</t>
         </is>
@@ -1177,10 +1362,15 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
           <t>55,08</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="D35" t="inlineStr">
         <is>
           <t>0,60</t>
         </is>
@@ -1194,10 +1384,15 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
           <t>70,21</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="D36" t="inlineStr">
         <is>
           <t>0,60</t>
         </is>
@@ -1211,15 +1406,20 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
           <t>76,51</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>0,60</t>
-        </is>
-      </c>
       <c r="D37" t="inlineStr">
+        <is>
+          <t>0,60</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
         <is>
           <t>0,56</t>
         </is>
@@ -1233,10 +1433,15 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
           <t>57,12</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
+      <c r="D38" t="inlineStr">
         <is>
           <t>0,40</t>
         </is>
@@ -1250,10 +1455,15 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
           <t>67,20</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="D39" t="inlineStr">
         <is>
           <t>0,40</t>
         </is>
@@ -1267,10 +1477,15 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
           <t>71,68</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="D40" t="inlineStr">
         <is>
           <t>0,40</t>
         </is>
@@ -1284,15 +1499,20 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
           <t>80,64</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>0,40</t>
-        </is>
-      </c>
       <c r="D41" t="inlineStr">
+        <is>
+          <t>0,40</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
         <is>
           <t>0,67</t>
         </is>
@@ -1306,10 +1526,15 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
           <t>85,91</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="D42" t="inlineStr">
         <is>
           <t>0,60</t>
         </is>
@@ -1323,10 +1548,15 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
           <t>101,07</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="D43" t="inlineStr">
         <is>
           <t>0,60</t>
         </is>
@@ -1340,10 +1570,15 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
           <t>105,37</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="D44" t="inlineStr">
         <is>
           <t>0,60</t>
         </is>
@@ -1357,15 +1592,20 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
           <t>118,27</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>0,60</t>
-        </is>
-      </c>
       <c r="D45" t="inlineStr">
+        <is>
+          <t>0,60</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
         <is>
           <t>1,08</t>
         </is>
@@ -1379,10 +1619,15 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
           <t>85,91</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="D46" t="inlineStr">
         <is>
           <t>0,60</t>
         </is>
@@ -1396,10 +1641,15 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
           <t>101,07</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="D47" t="inlineStr">
         <is>
           <t>0,60</t>
         </is>
@@ -1413,10 +1663,15 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
           <t>105,37</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
+      <c r="D48" t="inlineStr">
         <is>
           <t>0,60</t>
         </is>
@@ -1430,15 +1685,20 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
           <t>118,27</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>0,60</t>
-        </is>
-      </c>
       <c r="D49" t="inlineStr">
+        <is>
+          <t>0,60</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
         <is>
           <t>1,08</t>
         </is>
@@ -1452,10 +1712,15 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
           <t>85,91</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="D50" t="inlineStr">
         <is>
           <t>0,60</t>
         </is>
@@ -1469,10 +1734,15 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
           <t>101,07</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="D51" t="inlineStr">
         <is>
           <t>0,60</t>
         </is>
@@ -1486,10 +1756,15 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
           <t>105,37</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
+      <c r="D52" t="inlineStr">
         <is>
           <t>0,60</t>
         </is>
@@ -1503,15 +1778,20 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
           <t>118,27</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>0,60</t>
-        </is>
-      </c>
       <c r="D53" t="inlineStr">
+        <is>
+          <t>0,60</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
         <is>
           <t>1,08</t>
         </is>

</xml_diff>